<commit_message>
Update schedule file: Y4_B2526_General_&_Special_surgery_1_schedule.xlsx
</commit_message>
<xml_diff>
--- a/modules_schedules/Y4_B2526_General_&_Special_surgery_1_schedule.xlsx
+++ b/modules_schedules/Y4_B2526_General_&_Special_surgery_1_schedule.xlsx
@@ -463,7 +463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1427,6 +1427,2771 @@
         <v>180</v>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B28" s="2" t="inlineStr">
+        <is>
+          <t>B2D</t>
+        </is>
+      </c>
+      <c r="C28" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D28" s="2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E28" s="3" t="inlineStr">
+        <is>
+          <t>09/09/2025</t>
+        </is>
+      </c>
+      <c r="F28" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G28" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B29" s="6" t="inlineStr">
+        <is>
+          <t>B2D</t>
+        </is>
+      </c>
+      <c r="C29" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D29" s="6" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E29" s="7" t="inlineStr">
+        <is>
+          <t>10/09/2025</t>
+        </is>
+      </c>
+      <c r="F29" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G29" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B30" s="2" t="inlineStr">
+        <is>
+          <t>B2D</t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E30" s="3" t="inlineStr">
+        <is>
+          <t>11/09/2025</t>
+        </is>
+      </c>
+      <c r="F30" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G30" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B31" s="6" t="inlineStr">
+        <is>
+          <t>B2D</t>
+        </is>
+      </c>
+      <c r="C31" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D31" s="6" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E31" s="7" t="inlineStr">
+        <is>
+          <t>16/09/2025</t>
+        </is>
+      </c>
+      <c r="F31" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G31" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B32" s="2" t="inlineStr">
+        <is>
+          <t>B2D</t>
+        </is>
+      </c>
+      <c r="C32" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E32" s="3" t="inlineStr">
+        <is>
+          <t>17/09/2025</t>
+        </is>
+      </c>
+      <c r="F32" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G32" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B33" s="6" t="inlineStr">
+        <is>
+          <t>B2D</t>
+        </is>
+      </c>
+      <c r="C33" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D33" s="6" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E33" s="7" t="inlineStr">
+        <is>
+          <t>18/09/2025</t>
+        </is>
+      </c>
+      <c r="F33" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G33" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B34" s="2" t="inlineStr">
+        <is>
+          <t>B2D</t>
+        </is>
+      </c>
+      <c r="C34" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E34" s="3" t="inlineStr">
+        <is>
+          <t>23/09/2025</t>
+        </is>
+      </c>
+      <c r="F34" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G34" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B35" s="6" t="inlineStr">
+        <is>
+          <t>B2D</t>
+        </is>
+      </c>
+      <c r="C35" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D35" s="6" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E35" s="7" t="inlineStr">
+        <is>
+          <t>24/09/2025</t>
+        </is>
+      </c>
+      <c r="F35" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G35" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B36" s="2" t="inlineStr">
+        <is>
+          <t>B2D</t>
+        </is>
+      </c>
+      <c r="C36" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D36" s="2" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="E36" s="3" t="inlineStr">
+        <is>
+          <t>25/09/2025</t>
+        </is>
+      </c>
+      <c r="F36" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G36" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B37" s="6" t="inlineStr">
+        <is>
+          <t>B2D</t>
+        </is>
+      </c>
+      <c r="C37" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D37" s="6" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E37" s="7" t="inlineStr">
+        <is>
+          <t>30/09/2025</t>
+        </is>
+      </c>
+      <c r="F37" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G37" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B38" s="2" t="inlineStr">
+        <is>
+          <t>B2D</t>
+        </is>
+      </c>
+      <c r="C38" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D38" s="2" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E38" s="3" t="inlineStr">
+        <is>
+          <t>01/10/2025</t>
+        </is>
+      </c>
+      <c r="F38" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G38" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B39" s="6" t="inlineStr">
+        <is>
+          <t>B2D</t>
+        </is>
+      </c>
+      <c r="C39" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D39" s="6" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E39" s="7" t="inlineStr">
+        <is>
+          <t>02/10/2025</t>
+        </is>
+      </c>
+      <c r="F39" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G39" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B40" s="2" t="inlineStr">
+        <is>
+          <t>B2D</t>
+        </is>
+      </c>
+      <c r="C40" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D40" s="2" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E40" s="3" t="inlineStr">
+        <is>
+          <t>07/10/2025</t>
+        </is>
+      </c>
+      <c r="F40" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G40" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B41" s="6" t="inlineStr">
+        <is>
+          <t>B2D</t>
+        </is>
+      </c>
+      <c r="C41" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D41" s="6" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E41" s="7" t="inlineStr">
+        <is>
+          <t>08/10/2025</t>
+        </is>
+      </c>
+      <c r="F41" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G41" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B42" s="2" t="inlineStr">
+        <is>
+          <t>B2D</t>
+        </is>
+      </c>
+      <c r="C42" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D42" s="2" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E42" s="3" t="inlineStr">
+        <is>
+          <t>09/10/2025</t>
+        </is>
+      </c>
+      <c r="F42" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G42" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B43" s="6" t="inlineStr">
+        <is>
+          <t>B2D</t>
+        </is>
+      </c>
+      <c r="C43" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D43" s="6" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="E43" s="7" t="inlineStr">
+        <is>
+          <t>14/10/2025</t>
+        </is>
+      </c>
+      <c r="F43" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G43" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B44" s="2" t="inlineStr">
+        <is>
+          <t>B2D</t>
+        </is>
+      </c>
+      <c r="C44" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D44" s="2" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="E44" s="3" t="inlineStr">
+        <is>
+          <t>15/10/2025</t>
+        </is>
+      </c>
+      <c r="F44" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G44" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B45" s="6" t="inlineStr">
+        <is>
+          <t>B2D</t>
+        </is>
+      </c>
+      <c r="C45" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D45" s="6" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="E45" s="7" t="inlineStr">
+        <is>
+          <t>16/10/2025</t>
+        </is>
+      </c>
+      <c r="F45" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G45" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B46" s="2" t="inlineStr">
+        <is>
+          <t>B2D</t>
+        </is>
+      </c>
+      <c r="C46" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D46" s="2" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="E46" s="3" t="inlineStr">
+        <is>
+          <t>21/10/2025</t>
+        </is>
+      </c>
+      <c r="F46" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G46" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B47" s="6" t="inlineStr">
+        <is>
+          <t>B2D</t>
+        </is>
+      </c>
+      <c r="C47" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D47" s="6" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="E47" s="7" t="inlineStr">
+        <is>
+          <t>22/10/2025</t>
+        </is>
+      </c>
+      <c r="F47" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G47" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B48" s="2" t="inlineStr">
+        <is>
+          <t>B2D</t>
+        </is>
+      </c>
+      <c r="C48" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D48" s="2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="E48" s="3" t="inlineStr">
+        <is>
+          <t>23/10/2025</t>
+        </is>
+      </c>
+      <c r="F48" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G48" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B49" s="6" t="inlineStr">
+        <is>
+          <t>B2D</t>
+        </is>
+      </c>
+      <c r="C49" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D49" s="6" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="E49" s="7" t="inlineStr">
+        <is>
+          <t>28/10/2025</t>
+        </is>
+      </c>
+      <c r="F49" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G49" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B50" s="2" t="inlineStr">
+        <is>
+          <t>B2D</t>
+        </is>
+      </c>
+      <c r="C50" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D50" s="2" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="E50" s="3" t="inlineStr">
+        <is>
+          <t>29/10/2025</t>
+        </is>
+      </c>
+      <c r="F50" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G50" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B51" s="6" t="inlineStr">
+        <is>
+          <t>B2D</t>
+        </is>
+      </c>
+      <c r="C51" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D51" s="6" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="E51" s="7" t="inlineStr">
+        <is>
+          <t>30/10/2025</t>
+        </is>
+      </c>
+      <c r="F51" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G51" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B52" s="2" t="inlineStr">
+        <is>
+          <t>B2D</t>
+        </is>
+      </c>
+      <c r="C52" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D52" s="2" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="E52" s="3" t="inlineStr">
+        <is>
+          <t>04/11/2025</t>
+        </is>
+      </c>
+      <c r="F52" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G52" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B53" s="6" t="inlineStr">
+        <is>
+          <t>B2D</t>
+        </is>
+      </c>
+      <c r="C53" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D53" s="6" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="E53" s="7" t="inlineStr">
+        <is>
+          <t>05/11/2025</t>
+        </is>
+      </c>
+      <c r="F53" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G53" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B54" s="2" t="inlineStr">
+        <is>
+          <t>B2D</t>
+        </is>
+      </c>
+      <c r="C54" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D54" s="2" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="E54" s="3" t="inlineStr">
+        <is>
+          <t>06/11/2025</t>
+        </is>
+      </c>
+      <c r="F54" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G54" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B55" s="6" t="inlineStr">
+        <is>
+          <t>B2b</t>
+        </is>
+      </c>
+      <c r="C55" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D55" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E55" s="7" t="inlineStr">
+        <is>
+          <t>06/09/2025</t>
+        </is>
+      </c>
+      <c r="F55" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G55" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B56" s="2" t="inlineStr">
+        <is>
+          <t>B2b</t>
+        </is>
+      </c>
+      <c r="C56" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D56" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E56" s="3" t="inlineStr">
+        <is>
+          <t>07/09/2025</t>
+        </is>
+      </c>
+      <c r="F56" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G56" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B57" s="6" t="inlineStr">
+        <is>
+          <t>B2b</t>
+        </is>
+      </c>
+      <c r="C57" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D57" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E57" s="7" t="inlineStr">
+        <is>
+          <t>13/09/2025</t>
+        </is>
+      </c>
+      <c r="F57" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G57" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B58" s="2" t="inlineStr">
+        <is>
+          <t>B2b</t>
+        </is>
+      </c>
+      <c r="C58" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D58" s="2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E58" s="3" t="inlineStr">
+        <is>
+          <t>14/09/2025</t>
+        </is>
+      </c>
+      <c r="F58" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G58" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B59" s="6" t="inlineStr">
+        <is>
+          <t>B2b</t>
+        </is>
+      </c>
+      <c r="C59" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D59" s="6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E59" s="7" t="inlineStr">
+        <is>
+          <t>15/09/2025</t>
+        </is>
+      </c>
+      <c r="F59" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G59" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B60" s="2" t="inlineStr">
+        <is>
+          <t>B2b</t>
+        </is>
+      </c>
+      <c r="C60" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D60" s="2" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E60" s="3" t="inlineStr">
+        <is>
+          <t>20/09/2025</t>
+        </is>
+      </c>
+      <c r="F60" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G60" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B61" s="6" t="inlineStr">
+        <is>
+          <t>B2b</t>
+        </is>
+      </c>
+      <c r="C61" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D61" s="6" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E61" s="7" t="inlineStr">
+        <is>
+          <t>21/09/2025</t>
+        </is>
+      </c>
+      <c r="F61" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G61" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B62" s="2" t="inlineStr">
+        <is>
+          <t>B2b</t>
+        </is>
+      </c>
+      <c r="C62" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D62" s="2" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E62" s="3" t="inlineStr">
+        <is>
+          <t>22/09/2025</t>
+        </is>
+      </c>
+      <c r="F62" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G62" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B63" s="6" t="inlineStr">
+        <is>
+          <t>B2b</t>
+        </is>
+      </c>
+      <c r="C63" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D63" s="6" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="E63" s="7" t="inlineStr">
+        <is>
+          <t>27/09/2025</t>
+        </is>
+      </c>
+      <c r="F63" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G63" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B64" s="2" t="inlineStr">
+        <is>
+          <t>B2b</t>
+        </is>
+      </c>
+      <c r="C64" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D64" s="2" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E64" s="3" t="inlineStr">
+        <is>
+          <t>28/09/2025</t>
+        </is>
+      </c>
+      <c r="F64" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G64" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B65" s="6" t="inlineStr">
+        <is>
+          <t>B2b</t>
+        </is>
+      </c>
+      <c r="C65" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D65" s="6" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E65" s="7" t="inlineStr">
+        <is>
+          <t>29/09/2025</t>
+        </is>
+      </c>
+      <c r="F65" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G65" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B66" s="2" t="inlineStr">
+        <is>
+          <t>B2b</t>
+        </is>
+      </c>
+      <c r="C66" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D66" s="2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E66" s="3" t="inlineStr">
+        <is>
+          <t>04/10/2025</t>
+        </is>
+      </c>
+      <c r="F66" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G66" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B67" s="6" t="inlineStr">
+        <is>
+          <t>B2b</t>
+        </is>
+      </c>
+      <c r="C67" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D67" s="6" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E67" s="7" t="inlineStr">
+        <is>
+          <t>05/10/2025</t>
+        </is>
+      </c>
+      <c r="F67" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G67" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B68" s="2" t="inlineStr">
+        <is>
+          <t>B2b</t>
+        </is>
+      </c>
+      <c r="C68" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D68" s="2" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E68" s="3" t="inlineStr">
+        <is>
+          <t>06/10/2025</t>
+        </is>
+      </c>
+      <c r="F68" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G68" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B69" s="6" t="inlineStr">
+        <is>
+          <t>B2b</t>
+        </is>
+      </c>
+      <c r="C69" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D69" s="6" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E69" s="7" t="inlineStr">
+        <is>
+          <t>11/10/2025</t>
+        </is>
+      </c>
+      <c r="F69" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G69" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B70" s="2" t="inlineStr">
+        <is>
+          <t>B2b</t>
+        </is>
+      </c>
+      <c r="C70" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D70" s="2" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="E70" s="3" t="inlineStr">
+        <is>
+          <t>12/10/2025</t>
+        </is>
+      </c>
+      <c r="F70" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G70" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B71" s="6" t="inlineStr">
+        <is>
+          <t>B2b</t>
+        </is>
+      </c>
+      <c r="C71" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D71" s="6" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="E71" s="7" t="inlineStr">
+        <is>
+          <t>13/10/2025</t>
+        </is>
+      </c>
+      <c r="F71" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G71" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B72" s="2" t="inlineStr">
+        <is>
+          <t>B2b</t>
+        </is>
+      </c>
+      <c r="C72" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D72" s="2" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="E72" s="3" t="inlineStr">
+        <is>
+          <t>18/10/2025</t>
+        </is>
+      </c>
+      <c r="F72" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G72" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B73" s="6" t="inlineStr">
+        <is>
+          <t>B2b</t>
+        </is>
+      </c>
+      <c r="C73" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D73" s="6" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="E73" s="7" t="inlineStr">
+        <is>
+          <t>19/10/2025</t>
+        </is>
+      </c>
+      <c r="F73" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G73" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B74" s="2" t="inlineStr">
+        <is>
+          <t>B2b</t>
+        </is>
+      </c>
+      <c r="C74" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D74" s="2" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="E74" s="3" t="inlineStr">
+        <is>
+          <t>20/10/2025</t>
+        </is>
+      </c>
+      <c r="F74" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G74" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B75" s="6" t="inlineStr">
+        <is>
+          <t>B2b</t>
+        </is>
+      </c>
+      <c r="C75" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D75" s="6" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="E75" s="7" t="inlineStr">
+        <is>
+          <t>25/10/2025</t>
+        </is>
+      </c>
+      <c r="F75" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G75" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B76" s="2" t="inlineStr">
+        <is>
+          <t>B2b</t>
+        </is>
+      </c>
+      <c r="C76" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D76" s="2" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="E76" s="3" t="inlineStr">
+        <is>
+          <t>26/10/2025</t>
+        </is>
+      </c>
+      <c r="F76" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G76" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B77" s="6" t="inlineStr">
+        <is>
+          <t>B2b</t>
+        </is>
+      </c>
+      <c r="C77" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D77" s="6" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="E77" s="7" t="inlineStr">
+        <is>
+          <t>27/10/2025</t>
+        </is>
+      </c>
+      <c r="F77" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G77" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B78" s="2" t="inlineStr">
+        <is>
+          <t>B2b</t>
+        </is>
+      </c>
+      <c r="C78" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D78" s="2" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="E78" s="3" t="inlineStr">
+        <is>
+          <t>01/11/2025</t>
+        </is>
+      </c>
+      <c r="F78" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G78" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B79" s="6" t="inlineStr">
+        <is>
+          <t>B2b</t>
+        </is>
+      </c>
+      <c r="C79" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D79" s="6" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="E79" s="7" t="inlineStr">
+        <is>
+          <t>02/11/2025</t>
+        </is>
+      </c>
+      <c r="F79" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G79" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B80" s="2" t="inlineStr">
+        <is>
+          <t>B2b</t>
+        </is>
+      </c>
+      <c r="C80" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D80" s="2" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="E80" s="3" t="inlineStr">
+        <is>
+          <t>03/11/2025</t>
+        </is>
+      </c>
+      <c r="F80" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G80" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B81" s="6" t="inlineStr">
+        <is>
+          <t>B2c</t>
+        </is>
+      </c>
+      <c r="C81" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D81" s="6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E81" s="7" t="inlineStr">
+        <is>
+          <t>06/09/2025</t>
+        </is>
+      </c>
+      <c r="F81" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G81" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B82" s="2" t="inlineStr">
+        <is>
+          <t>B2c</t>
+        </is>
+      </c>
+      <c r="C82" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D82" s="2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E82" s="3" t="inlineStr">
+        <is>
+          <t>07/09/2025</t>
+        </is>
+      </c>
+      <c r="F82" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G82" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B83" s="6" t="inlineStr">
+        <is>
+          <t>B2c</t>
+        </is>
+      </c>
+      <c r="C83" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D83" s="6" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E83" s="7" t="inlineStr">
+        <is>
+          <t>13/09/2025</t>
+        </is>
+      </c>
+      <c r="F83" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G83" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B84" s="2" t="inlineStr">
+        <is>
+          <t>B2c</t>
+        </is>
+      </c>
+      <c r="C84" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D84" s="2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E84" s="3" t="inlineStr">
+        <is>
+          <t>14/09/2025</t>
+        </is>
+      </c>
+      <c r="F84" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G84" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B85" s="6" t="inlineStr">
+        <is>
+          <t>B2c</t>
+        </is>
+      </c>
+      <c r="C85" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D85" s="6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E85" s="7" t="inlineStr">
+        <is>
+          <t>15/09/2025</t>
+        </is>
+      </c>
+      <c r="F85" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G85" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B86" s="2" t="inlineStr">
+        <is>
+          <t>B2c</t>
+        </is>
+      </c>
+      <c r="C86" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D86" s="2" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E86" s="3" t="inlineStr">
+        <is>
+          <t>20/09/2025</t>
+        </is>
+      </c>
+      <c r="F86" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G86" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B87" s="6" t="inlineStr">
+        <is>
+          <t>B2c</t>
+        </is>
+      </c>
+      <c r="C87" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D87" s="6" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E87" s="7" t="inlineStr">
+        <is>
+          <t>21/09/2025</t>
+        </is>
+      </c>
+      <c r="F87" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G87" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B88" s="2" t="inlineStr">
+        <is>
+          <t>B2c</t>
+        </is>
+      </c>
+      <c r="C88" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D88" s="2" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E88" s="3" t="inlineStr">
+        <is>
+          <t>22/09/2025</t>
+        </is>
+      </c>
+      <c r="F88" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G88" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B89" s="6" t="inlineStr">
+        <is>
+          <t>B2c</t>
+        </is>
+      </c>
+      <c r="C89" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D89" s="6" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="E89" s="7" t="inlineStr">
+        <is>
+          <t>27/09/2025</t>
+        </is>
+      </c>
+      <c r="F89" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G89" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B90" s="2" t="inlineStr">
+        <is>
+          <t>B2c</t>
+        </is>
+      </c>
+      <c r="C90" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D90" s="2" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E90" s="3" t="inlineStr">
+        <is>
+          <t>28/09/2025</t>
+        </is>
+      </c>
+      <c r="F90" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G90" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B91" s="6" t="inlineStr">
+        <is>
+          <t>B2c</t>
+        </is>
+      </c>
+      <c r="C91" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D91" s="6" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E91" s="7" t="inlineStr">
+        <is>
+          <t>29/09/2025</t>
+        </is>
+      </c>
+      <c r="F91" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G91" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B92" s="2" t="inlineStr">
+        <is>
+          <t>B2c</t>
+        </is>
+      </c>
+      <c r="C92" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D92" s="2" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E92" s="3" t="inlineStr">
+        <is>
+          <t>04/10/2025</t>
+        </is>
+      </c>
+      <c r="F92" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G92" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B93" s="6" t="inlineStr">
+        <is>
+          <t>B2c</t>
+        </is>
+      </c>
+      <c r="C93" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D93" s="6" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E93" s="7" t="inlineStr">
+        <is>
+          <t>05/10/2025</t>
+        </is>
+      </c>
+      <c r="F93" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G93" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B94" s="2" t="inlineStr">
+        <is>
+          <t>B2c</t>
+        </is>
+      </c>
+      <c r="C94" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D94" s="2" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E94" s="3" t="inlineStr">
+        <is>
+          <t>06/10/2025</t>
+        </is>
+      </c>
+      <c r="F94" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G94" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B95" s="6" t="inlineStr">
+        <is>
+          <t>B2c</t>
+        </is>
+      </c>
+      <c r="C95" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D95" s="6" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E95" s="7" t="inlineStr">
+        <is>
+          <t>11/10/2025</t>
+        </is>
+      </c>
+      <c r="F95" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G95" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B96" s="2" t="inlineStr">
+        <is>
+          <t>B2c</t>
+        </is>
+      </c>
+      <c r="C96" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D96" s="2" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="E96" s="3" t="inlineStr">
+        <is>
+          <t>12/10/2025</t>
+        </is>
+      </c>
+      <c r="F96" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G96" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B97" s="6" t="inlineStr">
+        <is>
+          <t>B2c</t>
+        </is>
+      </c>
+      <c r="C97" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D97" s="6" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="E97" s="7" t="inlineStr">
+        <is>
+          <t>13/10/2025</t>
+        </is>
+      </c>
+      <c r="F97" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G97" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B98" s="2" t="inlineStr">
+        <is>
+          <t>B2c</t>
+        </is>
+      </c>
+      <c r="C98" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D98" s="2" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="E98" s="3" t="inlineStr">
+        <is>
+          <t>18/10/2025</t>
+        </is>
+      </c>
+      <c r="F98" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G98" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B99" s="6" t="inlineStr">
+        <is>
+          <t>B2c</t>
+        </is>
+      </c>
+      <c r="C99" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D99" s="6" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="E99" s="7" t="inlineStr">
+        <is>
+          <t>19/10/2025</t>
+        </is>
+      </c>
+      <c r="F99" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G99" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B100" s="2" t="inlineStr">
+        <is>
+          <t>B2c</t>
+        </is>
+      </c>
+      <c r="C100" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D100" s="2" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="E100" s="3" t="inlineStr">
+        <is>
+          <t>20/10/2025</t>
+        </is>
+      </c>
+      <c r="F100" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G100" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B101" s="6" t="inlineStr">
+        <is>
+          <t>B2c</t>
+        </is>
+      </c>
+      <c r="C101" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D101" s="6" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="E101" s="7" t="inlineStr">
+        <is>
+          <t>25/10/2025</t>
+        </is>
+      </c>
+      <c r="F101" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G101" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B102" s="2" t="inlineStr">
+        <is>
+          <t>B2c</t>
+        </is>
+      </c>
+      <c r="C102" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D102" s="2" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="E102" s="3" t="inlineStr">
+        <is>
+          <t>26/10/2025</t>
+        </is>
+      </c>
+      <c r="F102" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G102" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B103" s="6" t="inlineStr">
+        <is>
+          <t>B2c</t>
+        </is>
+      </c>
+      <c r="C103" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D103" s="6" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="E103" s="7" t="inlineStr">
+        <is>
+          <t>27/10/2025</t>
+        </is>
+      </c>
+      <c r="F103" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G103" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B104" s="2" t="inlineStr">
+        <is>
+          <t>B2c</t>
+        </is>
+      </c>
+      <c r="C104" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D104" s="2" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="E104" s="3" t="inlineStr">
+        <is>
+          <t>01/11/2025</t>
+        </is>
+      </c>
+      <c r="F104" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G104" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B105" s="6" t="inlineStr">
+        <is>
+          <t>B2c</t>
+        </is>
+      </c>
+      <c r="C105" s="6" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D105" s="6" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="E105" s="7" t="inlineStr">
+        <is>
+          <t>02/11/2025</t>
+        </is>
+      </c>
+      <c r="F105" s="8" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G105" s="9" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="2" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="B106" s="2" t="inlineStr">
+        <is>
+          <t>B2c</t>
+        </is>
+      </c>
+      <c r="C106" s="2" t="inlineStr">
+        <is>
+          <t>general surgery</t>
+        </is>
+      </c>
+      <c r="D106" s="2" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="E106" s="3" t="inlineStr">
+        <is>
+          <t>03/11/2025</t>
+        </is>
+      </c>
+      <c r="F106" s="4" t="inlineStr">
+        <is>
+          <t>10:30:00</t>
+        </is>
+      </c>
+      <c r="G106" s="5" t="n">
+        <v>180</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Upload Y4_B2526_General_&_Special_surgery_1_schedule.xlsx via attendance app
</commit_message>
<xml_diff>
--- a/modules_schedules/Y4_B2526_General_&_Special_surgery_1_schedule.xlsx
+++ b/modules_schedules/Y4_B2526_General_&_Special_surgery_1_schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moham\Desktop\modules_schedules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0226E57D-6DC3-4D53-A736-F2D4E2EEE5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7D492B-64A8-4BA6-86FC-0F9067B1222D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="580" windowWidth="18280" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1900" yWindow="580" windowWidth="18280" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General_&amp;_Special_surgery_1" sheetId="1" r:id="rId1"/>
@@ -362,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -386,9 +386,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="21" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -751,7 +748,7 @@
         <v>11</v>
       </c>
       <c r="G2" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -773,8 +770,8 @@
       <c r="F3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="9">
-        <v>180</v>
+      <c r="G3" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
@@ -797,7 +794,7 @@
         <v>11</v>
       </c>
       <c r="G4" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -819,8 +816,8 @@
       <c r="F5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="9">
-        <v>180</v>
+      <c r="G5" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -843,7 +840,7 @@
         <v>11</v>
       </c>
       <c r="G6" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -865,8 +862,8 @@
       <c r="F7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="9">
-        <v>180</v>
+      <c r="G7" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -889,7 +886,7 @@
         <v>11</v>
       </c>
       <c r="G8" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -911,8 +908,8 @@
       <c r="F9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="9">
-        <v>180</v>
+      <c r="G9" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -935,7 +932,7 @@
         <v>11</v>
       </c>
       <c r="G10" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -957,8 +954,8 @@
       <c r="F11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="9">
-        <v>180</v>
+      <c r="G11" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -981,7 +978,7 @@
         <v>11</v>
       </c>
       <c r="G12" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -1003,8 +1000,8 @@
       <c r="F13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="9">
-        <v>180</v>
+      <c r="G13" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
@@ -1027,7 +1024,7 @@
         <v>11</v>
       </c>
       <c r="G14" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -1049,8 +1046,8 @@
       <c r="F15" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="9">
-        <v>180</v>
+      <c r="G15" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -1073,7 +1070,7 @@
         <v>11</v>
       </c>
       <c r="G16" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
@@ -1095,8 +1092,8 @@
       <c r="F17" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="9">
-        <v>180</v>
+      <c r="G17" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -1119,7 +1116,7 @@
         <v>11</v>
       </c>
       <c r="G18" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
@@ -1141,8 +1138,8 @@
       <c r="F19" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="9">
-        <v>180</v>
+      <c r="G19" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.35">
@@ -1165,7 +1162,7 @@
         <v>11</v>
       </c>
       <c r="G20" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.35">
@@ -1187,8 +1184,8 @@
       <c r="F21" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G21" s="9">
-        <v>180</v>
+      <c r="G21" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -1211,7 +1208,7 @@
         <v>11</v>
       </c>
       <c r="G22" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
@@ -1233,8 +1230,8 @@
       <c r="F23" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G23" s="9">
-        <v>180</v>
+      <c r="G23" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
@@ -1257,7 +1254,7 @@
         <v>11</v>
       </c>
       <c r="G24" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -1279,8 +1276,8 @@
       <c r="F25" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G25" s="9">
-        <v>180</v>
+      <c r="G25" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
@@ -1303,7 +1300,7 @@
         <v>11</v>
       </c>
       <c r="G26" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
@@ -1325,8 +1322,8 @@
       <c r="F27" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G27" s="9">
-        <v>180</v>
+      <c r="G27" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
@@ -1349,7 +1346,7 @@
         <v>11</v>
       </c>
       <c r="G28" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
@@ -1371,8 +1368,8 @@
       <c r="F29" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G29" s="9">
-        <v>180</v>
+      <c r="G29" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
@@ -1395,7 +1392,7 @@
         <v>11</v>
       </c>
       <c r="G30" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
@@ -1417,8 +1414,8 @@
       <c r="F31" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G31" s="9">
-        <v>180</v>
+      <c r="G31" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
@@ -1441,7 +1438,7 @@
         <v>11</v>
       </c>
       <c r="G32" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
@@ -1463,8 +1460,8 @@
       <c r="F33" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G33" s="9">
-        <v>180</v>
+      <c r="G33" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
@@ -1487,7 +1484,7 @@
         <v>11</v>
       </c>
       <c r="G34" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
@@ -1509,8 +1506,8 @@
       <c r="F35" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G35" s="9">
-        <v>180</v>
+      <c r="G35" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
@@ -1533,7 +1530,7 @@
         <v>11</v>
       </c>
       <c r="G36" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
@@ -1555,8 +1552,8 @@
       <c r="F37" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G37" s="9">
-        <v>180</v>
+      <c r="G37" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
@@ -1579,7 +1576,7 @@
         <v>11</v>
       </c>
       <c r="G38" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.35">
@@ -1601,8 +1598,8 @@
       <c r="F39" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G39" s="9">
-        <v>180</v>
+      <c r="G39" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
@@ -1625,7 +1622,7 @@
         <v>11</v>
       </c>
       <c r="G40" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
@@ -1647,8 +1644,8 @@
       <c r="F41" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G41" s="9">
-        <v>180</v>
+      <c r="G41" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
@@ -1671,7 +1668,7 @@
         <v>11</v>
       </c>
       <c r="G42" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
@@ -1693,8 +1690,8 @@
       <c r="F43" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G43" s="9">
-        <v>180</v>
+      <c r="G43" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
@@ -1717,7 +1714,7 @@
         <v>11</v>
       </c>
       <c r="G44" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
@@ -1739,8 +1736,8 @@
       <c r="F45" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G45" s="9">
-        <v>180</v>
+      <c r="G45" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
@@ -1763,7 +1760,7 @@
         <v>11</v>
       </c>
       <c r="G46" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
@@ -1785,8 +1782,8 @@
       <c r="F47" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G47" s="9">
-        <v>180</v>
+      <c r="G47" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
@@ -1809,7 +1806,7 @@
         <v>11</v>
       </c>
       <c r="G48" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
@@ -1831,8 +1828,8 @@
       <c r="F49" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G49" s="9">
-        <v>180</v>
+      <c r="G49" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
@@ -1855,7 +1852,7 @@
         <v>11</v>
       </c>
       <c r="G50" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
@@ -1877,8 +1874,8 @@
       <c r="F51" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G51" s="9">
-        <v>180</v>
+      <c r="G51" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
@@ -1901,7 +1898,7 @@
         <v>11</v>
       </c>
       <c r="G52" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
@@ -1923,8 +1920,8 @@
       <c r="F53" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G53" s="9">
-        <v>180</v>
+      <c r="G53" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
@@ -1947,7 +1944,7 @@
         <v>11</v>
       </c>
       <c r="G54" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
@@ -1969,8 +1966,8 @@
       <c r="F55" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G55" s="9">
-        <v>180</v>
+      <c r="G55" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
@@ -1993,7 +1990,7 @@
         <v>11</v>
       </c>
       <c r="G56" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
@@ -2015,8 +2012,8 @@
       <c r="F57" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G57" s="9">
-        <v>180</v>
+      <c r="G57" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
@@ -2039,7 +2036,7 @@
         <v>11</v>
       </c>
       <c r="G58" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
@@ -2061,8 +2058,8 @@
       <c r="F59" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G59" s="9">
-        <v>180</v>
+      <c r="G59" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
@@ -2085,7 +2082,7 @@
         <v>11</v>
       </c>
       <c r="G60" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
@@ -2107,8 +2104,8 @@
       <c r="F61" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G61" s="9">
-        <v>180</v>
+      <c r="G61" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
@@ -2131,7 +2128,7 @@
         <v>11</v>
       </c>
       <c r="G62" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
@@ -2153,8 +2150,8 @@
       <c r="F63" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G63" s="9">
-        <v>180</v>
+      <c r="G63" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
@@ -2177,7 +2174,7 @@
         <v>11</v>
       </c>
       <c r="G64" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
@@ -2199,8 +2196,8 @@
       <c r="F65" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G65" s="9">
-        <v>180</v>
+      <c r="G65" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
@@ -2223,7 +2220,7 @@
         <v>11</v>
       </c>
       <c r="G66" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
@@ -2245,8 +2242,8 @@
       <c r="F67" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G67" s="9">
-        <v>180</v>
+      <c r="G67" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
@@ -2269,7 +2266,7 @@
         <v>11</v>
       </c>
       <c r="G68" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
@@ -2291,8 +2288,8 @@
       <c r="F69" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G69" s="9">
-        <v>180</v>
+      <c r="G69" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
@@ -2315,7 +2312,7 @@
         <v>11</v>
       </c>
       <c r="G70" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.35">
@@ -2337,8 +2334,8 @@
       <c r="F71" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G71" s="9">
-        <v>180</v>
+      <c r="G71" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.35">
@@ -2361,7 +2358,7 @@
         <v>11</v>
       </c>
       <c r="G72" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
@@ -2383,8 +2380,8 @@
       <c r="F73" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G73" s="9">
-        <v>180</v>
+      <c r="G73" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
@@ -2407,7 +2404,7 @@
         <v>11</v>
       </c>
       <c r="G74" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.35">
@@ -2429,8 +2426,8 @@
       <c r="F75" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G75" s="9">
-        <v>180</v>
+      <c r="G75" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.35">
@@ -2453,7 +2450,7 @@
         <v>11</v>
       </c>
       <c r="G76" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.35">
@@ -2475,8 +2472,8 @@
       <c r="F77" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G77" s="9">
-        <v>180</v>
+      <c r="G77" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.35">
@@ -2499,7 +2496,7 @@
         <v>11</v>
       </c>
       <c r="G78" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.35">
@@ -2521,8 +2518,8 @@
       <c r="F79" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G79" s="9">
-        <v>180</v>
+      <c r="G79" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
@@ -2545,7 +2542,7 @@
         <v>11</v>
       </c>
       <c r="G80" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.35">
@@ -2567,8 +2564,8 @@
       <c r="F81" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G81" s="9">
-        <v>180</v>
+      <c r="G81" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.35">
@@ -2591,7 +2588,7 @@
         <v>11</v>
       </c>
       <c r="G82" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
@@ -2613,8 +2610,8 @@
       <c r="F83" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G83" s="9">
-        <v>180</v>
+      <c r="G83" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.35">
@@ -2637,7 +2634,7 @@
         <v>11</v>
       </c>
       <c r="G84" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.35">
@@ -2659,8 +2656,8 @@
       <c r="F85" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G85" s="9">
-        <v>180</v>
+      <c r="G85" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
@@ -2683,7 +2680,7 @@
         <v>11</v>
       </c>
       <c r="G86" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.35">
@@ -2705,8 +2702,8 @@
       <c r="F87" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G87" s="9">
-        <v>180</v>
+      <c r="G87" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
@@ -2729,7 +2726,7 @@
         <v>11</v>
       </c>
       <c r="G88" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.35">
@@ -2751,8 +2748,8 @@
       <c r="F89" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G89" s="9">
-        <v>180</v>
+      <c r="G89" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.35">
@@ -2775,7 +2772,7 @@
         <v>11</v>
       </c>
       <c r="G90" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.35">
@@ -2797,8 +2794,8 @@
       <c r="F91" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G91" s="9">
-        <v>180</v>
+      <c r="G91" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.35">
@@ -2821,7 +2818,7 @@
         <v>11</v>
       </c>
       <c r="G92" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.35">
@@ -2843,8 +2840,8 @@
       <c r="F93" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G93" s="9">
-        <v>180</v>
+      <c r="G93" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.35">
@@ -2866,8 +2863,8 @@
       <c r="F94" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G94" s="9">
-        <v>180</v>
+      <c r="G94" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.35">
@@ -2890,7 +2887,7 @@
         <v>11</v>
       </c>
       <c r="G95" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.35">
@@ -2912,8 +2909,8 @@
       <c r="F96" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G96" s="9">
-        <v>180</v>
+      <c r="G96" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.35">
@@ -2936,7 +2933,7 @@
         <v>11</v>
       </c>
       <c r="G97" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.35">
@@ -2958,8 +2955,8 @@
       <c r="F98" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G98" s="9">
-        <v>180</v>
+      <c r="G98" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.35">
@@ -2982,7 +2979,7 @@
         <v>11</v>
       </c>
       <c r="G99" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.35">
@@ -3004,8 +3001,8 @@
       <c r="F100" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G100" s="9">
-        <v>180</v>
+      <c r="G100" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.35">
@@ -3028,7 +3025,7 @@
         <v>11</v>
       </c>
       <c r="G101" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.35">
@@ -3050,8 +3047,8 @@
       <c r="F102" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G102" s="9">
-        <v>180</v>
+      <c r="G102" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.35">
@@ -3074,7 +3071,7 @@
         <v>11</v>
       </c>
       <c r="G103" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.35">
@@ -3096,8 +3093,8 @@
       <c r="F104" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G104" s="9">
-        <v>180</v>
+      <c r="G104" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.35">
@@ -3120,7 +3117,7 @@
         <v>11</v>
       </c>
       <c r="G105" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.35">
@@ -3142,8 +3139,8 @@
       <c r="F106" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G106" s="9">
-        <v>180</v>
+      <c r="G106" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.35">
@@ -3166,7 +3163,7 @@
         <v>11</v>
       </c>
       <c r="G107" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.35">
@@ -3188,8 +3185,8 @@
       <c r="F108" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G108" s="9">
-        <v>180</v>
+      <c r="G108" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.35">
@@ -3212,7 +3209,7 @@
         <v>11</v>
       </c>
       <c r="G109" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.35">
@@ -3234,8 +3231,8 @@
       <c r="F110" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G110" s="9">
-        <v>180</v>
+      <c r="G110" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.35">
@@ -3258,7 +3255,7 @@
         <v>11</v>
       </c>
       <c r="G111" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.35">
@@ -3280,8 +3277,8 @@
       <c r="F112" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G112" s="9">
-        <v>180</v>
+      <c r="G112" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.35">
@@ -3304,7 +3301,7 @@
         <v>11</v>
       </c>
       <c r="G113" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.35">
@@ -3326,8 +3323,8 @@
       <c r="F114" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G114" s="9">
-        <v>180</v>
+      <c r="G114" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.35">
@@ -3350,7 +3347,7 @@
         <v>11</v>
       </c>
       <c r="G115" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.35">
@@ -3372,8 +3369,8 @@
       <c r="F116" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G116" s="9">
-        <v>180</v>
+      <c r="G116" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.35">
@@ -3396,7 +3393,7 @@
         <v>11</v>
       </c>
       <c r="G117" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.35">
@@ -3418,8 +3415,8 @@
       <c r="F118" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G118" s="9">
-        <v>180</v>
+      <c r="G118" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.35">
@@ -3442,7 +3439,7 @@
         <v>11</v>
       </c>
       <c r="G119" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.35">
@@ -3465,7 +3462,7 @@
         <v>11</v>
       </c>
       <c r="G120" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.35">
@@ -3487,8 +3484,8 @@
       <c r="F121" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G121" s="9">
-        <v>180</v>
+      <c r="G121" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.35">
@@ -3511,7 +3508,7 @@
         <v>11</v>
       </c>
       <c r="G122" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.35">
@@ -3533,8 +3530,8 @@
       <c r="F123" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G123" s="9">
-        <v>180</v>
+      <c r="G123" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.35">
@@ -3557,7 +3554,7 @@
         <v>11</v>
       </c>
       <c r="G124" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.35">
@@ -3579,8 +3576,8 @@
       <c r="F125" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G125" s="9">
-        <v>180</v>
+      <c r="G125" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.35">
@@ -3603,7 +3600,7 @@
         <v>11</v>
       </c>
       <c r="G126" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.35">
@@ -3625,8 +3622,8 @@
       <c r="F127" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G127" s="9">
-        <v>180</v>
+      <c r="G127" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.35">
@@ -3649,7 +3646,7 @@
         <v>11</v>
       </c>
       <c r="G128" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.35">
@@ -3671,8 +3668,8 @@
       <c r="F129" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G129" s="9">
-        <v>180</v>
+      <c r="G129" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.35">
@@ -3695,7 +3692,7 @@
         <v>11</v>
       </c>
       <c r="G130" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.35">
@@ -3717,8 +3714,8 @@
       <c r="F131" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G131" s="9">
-        <v>180</v>
+      <c r="G131" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.35">
@@ -3741,7 +3738,7 @@
         <v>0.4375</v>
       </c>
       <c r="G132" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.35">
@@ -3763,8 +3760,8 @@
       <c r="F133" s="8">
         <v>0.4375</v>
       </c>
-      <c r="G133" s="9">
-        <v>180</v>
+      <c r="G133" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.35">
@@ -3787,7 +3784,7 @@
         <v>0.4375</v>
       </c>
       <c r="G134" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.35">
@@ -3809,8 +3806,8 @@
       <c r="F135" s="8">
         <v>0.4375</v>
       </c>
-      <c r="G135" s="9">
-        <v>180</v>
+      <c r="G135" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.35">
@@ -3833,7 +3830,7 @@
         <v>0.4375</v>
       </c>
       <c r="G136" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.35">
@@ -3855,8 +3852,8 @@
       <c r="F137" s="8">
         <v>0.4375</v>
       </c>
-      <c r="G137" s="9">
-        <v>180</v>
+      <c r="G137" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.35">
@@ -3879,7 +3876,7 @@
         <v>0.4375</v>
       </c>
       <c r="G138" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.35">
@@ -3901,8 +3898,8 @@
       <c r="F139" s="8">
         <v>0.4375</v>
       </c>
-      <c r="G139" s="9">
-        <v>180</v>
+      <c r="G139" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.35">
@@ -3925,7 +3922,7 @@
         <v>0.4375</v>
       </c>
       <c r="G140" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.35">
@@ -3947,8 +3944,8 @@
       <c r="F141" s="8">
         <v>0.4375</v>
       </c>
-      <c r="G141" s="9">
-        <v>180</v>
+      <c r="G141" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.35">
@@ -3971,7 +3968,7 @@
         <v>0.4375</v>
       </c>
       <c r="G142" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.35">
@@ -3993,8 +3990,8 @@
       <c r="F143" s="8">
         <v>0.4375</v>
       </c>
-      <c r="G143" s="9">
-        <v>180</v>
+      <c r="G143" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.35">
@@ -4017,7 +4014,7 @@
         <v>0.4375</v>
       </c>
       <c r="G144" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.35">
@@ -4039,8 +4036,8 @@
       <c r="F145" s="8">
         <v>0.4375</v>
       </c>
-      <c r="G145" s="9">
-        <v>180</v>
+      <c r="G145" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.35">
@@ -4062,8 +4059,8 @@
       <c r="F146" s="8">
         <v>0.4375</v>
       </c>
-      <c r="G146" s="9">
-        <v>180</v>
+      <c r="G146" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.35">
@@ -4086,7 +4083,7 @@
         <v>0.4375</v>
       </c>
       <c r="G147" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.35">
@@ -4108,8 +4105,8 @@
       <c r="F148" s="8">
         <v>0.4375</v>
       </c>
-      <c r="G148" s="9">
-        <v>180</v>
+      <c r="G148" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.35">
@@ -4132,7 +4129,7 @@
         <v>0.4375</v>
       </c>
       <c r="G149" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.35">
@@ -4154,8 +4151,8 @@
       <c r="F150" s="8">
         <v>0.4375</v>
       </c>
-      <c r="G150" s="9">
-        <v>180</v>
+      <c r="G150" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.35">
@@ -4178,7 +4175,7 @@
         <v>0.4375</v>
       </c>
       <c r="G151" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.35">
@@ -4200,8 +4197,8 @@
       <c r="F152" s="8">
         <v>0.4375</v>
       </c>
-      <c r="G152" s="9">
-        <v>180</v>
+      <c r="G152" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.35">
@@ -4224,7 +4221,7 @@
         <v>0.4375</v>
       </c>
       <c r="G153" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.35">
@@ -4246,8 +4243,8 @@
       <c r="F154" s="8">
         <v>0.4375</v>
       </c>
-      <c r="G154" s="9">
-        <v>180</v>
+      <c r="G154" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.35">
@@ -4270,7 +4267,7 @@
         <v>0.4375</v>
       </c>
       <c r="G155" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.35">
@@ -4292,8 +4289,8 @@
       <c r="F156" s="8">
         <v>0.4375</v>
       </c>
-      <c r="G156" s="9">
-        <v>180</v>
+      <c r="G156" s="5">
+        <v>90</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.35">
@@ -4316,7 +4313,7 @@
         <v>0.4375</v>
       </c>
       <c r="G157" s="5">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>